<commit_message>
Se completa presupuesto con su justificación y el flujo de caja
</commit_message>
<xml_diff>
--- a/Proyecto/Primera Entrega/Documentos/(SnoutPoint) Flujo de caja.xlsx
+++ b/Proyecto/Primera Entrega/Documentos/(SnoutPoint) Flujo de caja.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="48" windowWidth="22116" windowHeight="9552"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="(SnoutPoint) Flujo de Caja" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Desarrollar el proyecto sobre 6 periodos (meses) desde el periodo 0 hasta el periodo 5</t>
   </si>
@@ -27,24 +27,9 @@
     <t>costos de ventas equivalentes a 0$ de las ventas</t>
   </si>
   <si>
-    <t>Costos de entrega de los activos fijos</t>
-  </si>
-  <si>
-    <t>Costos de instalación de los activos fijos</t>
-  </si>
-  <si>
-    <t>Cobertura de seguro</t>
-  </si>
-  <si>
-    <t>Entrenamiento del personal</t>
-  </si>
-  <si>
     <t xml:space="preserve">otros costos de $200.000 en el periodo 0, luego equivalentes al 30% del costo inicial </t>
   </si>
   <si>
-    <t>valor de rescate 0$, debido a que no se venderan los equipos al final</t>
-  </si>
-  <si>
     <t>tasa impositiva de 30%</t>
   </si>
   <si>
@@ -129,9 +114,6 @@
     <t>Depreciación por periodo</t>
   </si>
   <si>
-    <t>inversion inicial en:</t>
-  </si>
-  <si>
     <t>HP Pavilion G6</t>
   </si>
   <si>
@@ -213,10 +195,19 @@
     <t>Desinversión:</t>
   </si>
   <si>
-    <t xml:space="preserve">con un valor de </t>
-  </si>
-  <si>
-    <t>hasta el periodo 5</t>
+    <t>valor de rescate 0$, debido a que no se venderán los equipos al final</t>
+  </si>
+  <si>
+    <t>inversión inicial en:</t>
+  </si>
+  <si>
+    <t>hasta el periodo 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para el periodo 0, y un valor de </t>
+  </si>
+  <si>
+    <t>Tasa de oportunidad:</t>
   </si>
 </sst>
 </file>
@@ -226,7 +217,7 @@
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -285,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +313,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="43">
     <border>
@@ -883,7 +880,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -927,37 +924,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1092,19 +1089,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1119,40 +1116,40 @@
     <xf numFmtId="10" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1161,19 +1158,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1185,11 +1182,20 @@
     <xf numFmtId="8" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1496,16 +1502,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5546875" style="2" customWidth="1"/>
@@ -1534,66 +1540,54 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B5" s="10">
         <f>H39</f>
         <v>4600000</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B9" s="10">
         <v>10000000</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
+      <c r="C9" s="103" t="s">
+        <v>62</v>
       </c>
       <c r="D9" s="10">
         <v>500000</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" s="32">
         <f>1/36</f>
@@ -1602,7 +1596,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12" s="33">
         <f>H39</f>
@@ -1611,7 +1605,7 @@
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" s="34">
         <f>B12*B11</f>
@@ -1623,12 +1617,12 @@
     </row>
     <row r="15" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B16" s="98">
         <v>0</v>
@@ -1652,7 +1646,7 @@
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -1676,7 +1670,7 @@
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B18" s="18">
         <v>0</v>
@@ -1700,7 +1694,7 @@
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B19" s="18">
         <v>200000</v>
@@ -1729,7 +1723,7 @@
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -1758,7 +1752,7 @@
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B21" s="18">
         <f>B17-B18-B19-B20</f>
@@ -1788,7 +1782,7 @@
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B22" s="18">
         <f>B21*0.3</f>
@@ -1818,7 +1812,7 @@
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B23" s="18">
         <f>B17-B18-B19-B22</f>
@@ -1848,7 +1842,7 @@
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B24" s="18">
         <f>B53</f>
@@ -1878,7 +1872,7 @@
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B25" s="18">
         <f>B54</f>
@@ -1908,7 +1902,7 @@
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="92" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B26" s="93">
         <f>-B5</f>
@@ -1934,7 +1928,7 @@
     </row>
     <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="91" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B27" s="96">
         <f>B23+B25-B26</f>
@@ -1965,49 +1959,55 @@
     <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="99" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B29" s="100">
-        <f>NPV(10%,C27:G27)+B27</f>
-        <v>2678865.2248873534</v>
+        <f>NPV(E29,C27:G27)+B27</f>
+        <v>1583697.9869447229</v>
+      </c>
+      <c r="D29" s="104" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="105">
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:8" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="36" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B31" s="35" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G31" s="36" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H31" s="36" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B32" s="41">
         <v>900000</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D32" s="43">
         <v>2012</v>
@@ -2029,13 +2029,13 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B33" s="47">
         <v>1500000</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D33" s="49">
         <v>2013</v>
@@ -2057,13 +2057,13 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B34" s="54">
         <v>1200000</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D34" s="49">
         <v>2013</v>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B35" s="54">
         <v>900000</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D35" s="56">
         <v>2013</v>
@@ -2113,13 +2113,13 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B36" s="54">
         <v>1300000</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D36" s="49">
         <v>2012</v>
@@ -2141,13 +2141,13 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B37" s="54">
         <v>1000000</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D37" s="49">
         <v>2012</v>
@@ -2169,13 +2169,13 @@
     </row>
     <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B38" s="58">
         <v>1000000</v>
       </c>
       <c r="C38" s="59" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D38" s="60">
         <v>2012</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B39" s="65">
         <f>SUM(B32:B38)</f>
@@ -2218,20 +2218,20 @@
     </row>
     <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B40" s="87" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G42" s="40" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B43" s="13">
         <v>0</v>
@@ -2261,7 +2261,7 @@
         <v>8</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L43" s="13">
         <v>36</v>
@@ -2269,86 +2269,86 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B44" s="75">
-        <f>$B$11</f>
+        <f t="shared" ref="B44:G44" si="8">$B$11</f>
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="C44" s="76">
-        <f>$B$11</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="D44" s="76">
-        <f>$B$11</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="E44" s="76">
-        <f>$B$11</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="F44" s="77">
-        <f>$B$11</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="G44" s="78">
-        <f>$B$11</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="H44" s="76">
-        <f t="shared" ref="H44:L44" si="8">$B$11</f>
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="I44" s="77">
         <f t="shared" si="8"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="J44" s="67">
+      <c r="D44" s="76">
         <f t="shared" si="8"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="K44" s="68" t="s">
-        <v>62</v>
-      </c>
-      <c r="L44" s="69">
+      <c r="E44" s="76">
         <f t="shared" si="8"/>
         <v>2.7777777777777776E-2</v>
       </c>
+      <c r="F44" s="77">
+        <f t="shared" si="8"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G44" s="78">
+        <f t="shared" si="8"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="H44" s="76">
+        <f t="shared" ref="H44:L44" si="9">$B$11</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="I44" s="77">
+        <f t="shared" si="9"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="J44" s="67">
+        <f t="shared" si="9"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="K44" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="L44" s="69">
+        <f t="shared" si="9"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B45" s="79">
-        <f>$B$13</f>
+        <f t="shared" ref="B45:G45" si="10">$B$13</f>
         <v>127777.77777777777</v>
       </c>
       <c r="C45" s="80">
-        <f>$B$13</f>
+        <f t="shared" si="10"/>
         <v>127777.77777777777</v>
       </c>
       <c r="D45" s="80">
-        <f>$B$13</f>
+        <f t="shared" si="10"/>
         <v>127777.77777777777</v>
       </c>
       <c r="E45" s="80">
-        <f>$B$13</f>
+        <f t="shared" si="10"/>
         <v>127777.77777777777</v>
       </c>
       <c r="F45" s="81">
-        <f>$B$13</f>
+        <f t="shared" si="10"/>
         <v>127777.77777777777</v>
       </c>
       <c r="G45" s="82">
-        <f>$B$13</f>
+        <f t="shared" si="10"/>
         <v>127777.77777777777</v>
       </c>
       <c r="H45" s="80">
-        <f t="shared" ref="H45:I45" si="9">$B$13</f>
+        <f t="shared" ref="H45:I45" si="11">$B$13</f>
         <v>127777.77777777777</v>
       </c>
       <c r="I45" s="81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>127777.77777777777</v>
       </c>
       <c r="J45" s="70">
@@ -2356,7 +2356,7 @@
         <v>127777.77777777777</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L45" s="71">
         <f>$B$13</f>
@@ -2365,46 +2365,46 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B46" s="79">
         <f>B45</f>
         <v>127777.77777777777</v>
       </c>
       <c r="C46" s="80">
-        <f>B46+C45</f>
+        <f t="shared" ref="C46:J46" si="12">B46+C45</f>
         <v>255555.55555555553</v>
       </c>
       <c r="D46" s="80">
-        <f>C46+D45</f>
+        <f t="shared" si="12"/>
         <v>383333.33333333331</v>
       </c>
       <c r="E46" s="80">
-        <f>D46+E45</f>
+        <f t="shared" si="12"/>
         <v>511111.11111111107</v>
       </c>
       <c r="F46" s="81">
-        <f>E46+F45</f>
+        <f t="shared" si="12"/>
         <v>638888.88888888888</v>
       </c>
       <c r="G46" s="82">
-        <f>F46+G45</f>
+        <f t="shared" si="12"/>
         <v>766666.66666666663</v>
       </c>
       <c r="H46" s="80">
-        <f>G46+H45</f>
+        <f t="shared" si="12"/>
         <v>894444.44444444438</v>
       </c>
       <c r="I46" s="81">
-        <f>H46+I45</f>
+        <f t="shared" si="12"/>
         <v>1022222.2222222221</v>
       </c>
       <c r="J46" s="70">
-        <f>I46+J45</f>
+        <f t="shared" si="12"/>
         <v>1150000</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L46" s="71">
         <f>B12</f>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B47" s="83">
         <f>B12-B45</f>
@@ -2452,7 +2452,7 @@
         <v>3450000</v>
       </c>
       <c r="K47" s="73" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L47" s="74">
         <f>0</f>
@@ -2481,7 +2481,7 @@
       <c r="E49" s="88"/>
       <c r="F49" s="88"/>
       <c r="G49" s="102" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H49" s="101">
         <f>0-0.3*(0-G47)</f>
@@ -2497,12 +2497,12 @@
     </row>
     <row r="51" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B52" s="13">
         <v>0</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="26" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B53" s="15">
         <v>10000000</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B54" s="21">
         <f>-B53</f>
@@ -2563,11 +2563,11 @@
         <v>0</v>
       </c>
       <c r="E54" s="22">
-        <f t="shared" ref="E54:G54" si="10">-E53+D53</f>
+        <f t="shared" ref="E54:F54" si="13">-E53+D53</f>
         <v>0</v>
       </c>
       <c r="F54" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G54" s="22">

</xml_diff>